<commit_message>
Added decimal places on population size
</commit_message>
<xml_diff>
--- a/tool/SUBsET Pakistan.xlsx
+++ b/tool/SUBsET Pakistan.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10714"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aschwalbc/Documents/Research/SUBsET-PAK/tool/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA24465C-89A5-A648-99A8-845ACE60CA4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED58267A-AAAE-1F49-B4E2-B867AA856CDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="880" windowWidth="25160" windowHeight="22500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1442,9 +1442,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.0000"/>
+    <numFmt numFmtId="166" formatCode="0.000"/>
   </numFmts>
   <fonts count="19" x14ac:knownFonts="1">
     <font>
@@ -2008,7 +2009,7 @@
     <xf numFmtId="43" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="190">
+  <cellXfs count="191">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2357,6 +2358,7 @@
     <xf numFmtId="0" fontId="4" fillId="19" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -24781,8 +24783,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{398A8C26-8181-BA4E-87BF-BF7D76B7F7F7}">
   <dimension ref="A1:U151"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G143" workbookViewId="0">
-      <selection activeCell="U152" sqref="U152"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2:F151"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -24883,7 +24885,7 @@
         <f>'Input 1'!F3</f>
         <v>591</v>
       </c>
-      <c r="F2" s="109">
+      <c r="F2" s="190">
         <f>Estimates!D3</f>
         <v>400.07100000000003</v>
       </c>
@@ -24969,7 +24971,7 @@
         <f>'Input 1'!F4</f>
         <v>741</v>
       </c>
-      <c r="F3" s="109">
+      <c r="F3" s="190">
         <f>Estimates!D4</f>
         <v>458.96499999999997</v>
       </c>
@@ -25055,7 +25057,7 @@
         <f>'Input 1'!F5</f>
         <v>273</v>
       </c>
-      <c r="F4" s="109">
+      <c r="F4" s="190">
         <f>Estimates!D5</f>
         <v>251.29499999999999</v>
       </c>
@@ -25141,7 +25143,7 @@
         <f>'Input 1'!F6</f>
         <v>167</v>
       </c>
-      <c r="F5" s="109">
+      <c r="F5" s="190">
         <f>Estimates!D6</f>
         <v>166.64400000000001</v>
       </c>
@@ -25227,7 +25229,7 @@
         <f>'Input 1'!F7</f>
         <v>655</v>
       </c>
-      <c r="F6" s="109">
+      <c r="F6" s="190">
         <f>Estimates!D7</f>
         <v>847.25699999999995</v>
       </c>
@@ -25313,7 +25315,7 @@
         <f>'Input 1'!F8</f>
         <v>503</v>
       </c>
-      <c r="F7" s="109">
+      <c r="F7" s="190">
         <f>Estimates!D8</f>
         <v>495.34300000000002</v>
       </c>
@@ -25399,7 +25401,7 @@
         <f>'Input 1'!F9</f>
         <v>853</v>
       </c>
-      <c r="F8" s="109">
+      <c r="F8" s="190">
         <f>Estimates!D9</f>
         <v>714.9</v>
       </c>
@@ -25485,7 +25487,7 @@
         <f>'Input 1'!F10</f>
         <v>168</v>
       </c>
-      <c r="F9" s="109">
+      <c r="F9" s="190">
         <f>Estimates!D10</f>
         <v>213.548</v>
       </c>
@@ -25571,7 +25573,7 @@
         <f>'Input 1'!F11</f>
         <v>382</v>
       </c>
-      <c r="F10" s="109">
+      <c r="F10" s="190">
         <f>Estimates!D11</f>
         <v>548.35</v>
       </c>
@@ -25657,7 +25659,7 @@
         <f>'Input 1'!F12</f>
         <v>284</v>
       </c>
-      <c r="F11" s="109">
+      <c r="F11" s="190">
         <f>Estimates!D12</f>
         <v>320.58199999999999</v>
       </c>
@@ -25743,7 +25745,7 @@
         <f>'Input 1'!F13</f>
         <v>52</v>
       </c>
-      <c r="F12" s="109">
+      <c r="F12" s="190">
         <f>Estimates!D13</f>
         <v>122.595</v>
       </c>
@@ -25829,7 +25831,7 @@
         <f>'Input 1'!F14</f>
         <v>64</v>
       </c>
-      <c r="F13" s="109">
+      <c r="F13" s="190">
         <f>Estimates!D14</f>
         <v>195.90600000000001</v>
       </c>
@@ -25915,7 +25917,7 @@
         <f>'Input 1'!F15</f>
         <v>135</v>
       </c>
-      <c r="F14" s="109">
+      <c r="F14" s="190">
         <f>Estimates!D15</f>
         <v>276.69600000000003</v>
       </c>
@@ -26001,7 +26003,7 @@
         <f>'Input 1'!F16</f>
         <v>69</v>
       </c>
-      <c r="F15" s="109">
+      <c r="F15" s="190">
         <f>Estimates!D16</f>
         <v>360.637</v>
       </c>
@@ -26087,7 +26089,7 @@
         <f>'Input 1'!F17</f>
         <v>54</v>
       </c>
-      <c r="F16" s="109">
+      <c r="F16" s="190">
         <f>Estimates!D17</f>
         <v>288.95</v>
       </c>
@@ -26173,7 +26175,7 @@
         <f>'Input 1'!F18</f>
         <v>17</v>
       </c>
-      <c r="F17" s="109">
+      <c r="F17" s="190">
         <f>Estimates!D18</f>
         <v>103.18300000000001</v>
       </c>
@@ -26259,7 +26261,7 @@
         <f>'Input 1'!F19</f>
         <v>804</v>
       </c>
-      <c r="F18" s="109">
+      <c r="F18" s="190">
         <f>Estimates!D19</f>
         <v>596.22900000000004</v>
       </c>
@@ -26345,7 +26347,7 @@
         <f>'Input 1'!F20</f>
         <v>578</v>
       </c>
-      <c r="F19" s="109">
+      <c r="F19" s="190">
         <f>Estimates!D20</f>
         <v>161.71</v>
       </c>
@@ -26431,7 +26433,7 @@
         <f>'Input 1'!F21</f>
         <v>67</v>
       </c>
-      <c r="F20" s="109">
+      <c r="F20" s="190">
         <f>Estimates!D21</f>
         <v>248.01300000000001</v>
       </c>
@@ -26517,7 +26519,7 @@
         <f>'Input 1'!F22</f>
         <v>59</v>
       </c>
-      <c r="F21" s="109">
+      <c r="F21" s="190">
         <f>Estimates!D22</f>
         <v>476.26799999999997</v>
       </c>
@@ -26603,7 +26605,7 @@
         <f>'Input 1'!F23</f>
         <v>232</v>
       </c>
-      <c r="F22" s="109">
+      <c r="F22" s="190">
         <f>Estimates!D23</f>
         <v>1118.364</v>
       </c>
@@ -26689,7 +26691,7 @@
         <f>'Input 1'!F24</f>
         <v>118</v>
       </c>
-      <c r="F23" s="109">
+      <c r="F23" s="190">
         <f>Estimates!D24</f>
         <v>177.017</v>
       </c>
@@ -26775,7 +26777,7 @@
         <f>'Input 1'!F25</f>
         <v>486</v>
       </c>
-      <c r="F24" s="109">
+      <c r="F24" s="190">
         <f>Estimates!D25</f>
         <v>952.31</v>
       </c>
@@ -26861,7 +26863,7 @@
         <f>'Input 1'!F26</f>
         <v>432</v>
       </c>
-      <c r="F25" s="109">
+      <c r="F25" s="190">
         <f>Estimates!D26</f>
         <v>920.38099999999997</v>
       </c>
@@ -26947,7 +26949,7 @@
         <f>'Input 1'!F27</f>
         <v>537</v>
       </c>
-      <c r="F26" s="109">
+      <c r="F26" s="190">
         <f>Estimates!D27</f>
         <v>398.38099999999997</v>
       </c>
@@ -27033,7 +27035,7 @@
         <f>'Input 1'!F28</f>
         <v>68</v>
       </c>
-      <c r="F27" s="109">
+      <c r="F27" s="190">
         <f>Estimates!D28</f>
         <v>261.92</v>
       </c>
@@ -27119,7 +27121,7 @@
         <f>'Input 1'!F29</f>
         <v>587</v>
       </c>
-      <c r="F28" s="109">
+      <c r="F28" s="190">
         <f>Estimates!D29</f>
         <v>673.55499999999995</v>
       </c>
@@ -27205,7 +27207,7 @@
         <f>'Input 1'!F30</f>
         <v>257</v>
       </c>
-      <c r="F29" s="109">
+      <c r="F29" s="190">
         <f>Estimates!D30</f>
         <v>448.745</v>
       </c>
@@ -27291,7 +27293,7 @@
         <f>'Input 1'!F31</f>
         <v>129</v>
       </c>
-      <c r="F30" s="109">
+      <c r="F30" s="190">
         <f>Estimates!D31</f>
         <v>309.50200000000001</v>
       </c>
@@ -27377,7 +27379,7 @@
         <f>'Input 1'!F32</f>
         <v>29</v>
       </c>
-      <c r="F31" s="109">
+      <c r="F31" s="190">
         <f>Estimates!D32</f>
         <v>176.93100000000001</v>
       </c>
@@ -27463,7 +27465,7 @@
         <f>'Input 1'!F33</f>
         <v>530</v>
       </c>
-      <c r="F32" s="109">
+      <c r="F32" s="190">
         <f>Estimates!D33</f>
         <v>587.97299999999996</v>
       </c>
@@ -27549,7 +27551,7 @@
         <f>'Input 1'!F34</f>
         <v>208</v>
       </c>
-      <c r="F33" s="109">
+      <c r="F33" s="190">
         <f>Estimates!D34</f>
         <v>209.39500000000001</v>
       </c>
@@ -27635,7 +27637,7 @@
         <f>'Input 1'!F35</f>
         <v>81</v>
       </c>
-      <c r="F34" s="109">
+      <c r="F34" s="190">
         <f>Estimates!D35</f>
         <v>342.51900000000001</v>
       </c>
@@ -27721,7 +27723,7 @@
         <f>'Input 1'!F36</f>
         <v>598</v>
       </c>
-      <c r="F35" s="109">
+      <c r="F35" s="190">
         <f>Estimates!D36</f>
         <v>878.09400000000005</v>
       </c>
@@ -27807,7 +27809,7 @@
         <f>'Input 1'!F37</f>
         <v>2962</v>
       </c>
-      <c r="F36" s="109">
+      <c r="F36" s="190">
         <f>Estimates!D37</f>
         <v>3021.056</v>
       </c>
@@ -27893,7 +27895,7 @@
         <f>'Input 1'!F38</f>
         <v>112</v>
       </c>
-      <c r="F37" s="109">
+      <c r="F37" s="190">
         <f>Estimates!D38</f>
         <v>180.54</v>
       </c>
@@ -27979,7 +27981,7 @@
         <f>'Input 1'!F39</f>
         <v>233</v>
       </c>
-      <c r="F38" s="109">
+      <c r="F38" s="190">
         <f>Estimates!D39</f>
         <v>145.40299999999999</v>
       </c>
@@ -28065,7 +28067,7 @@
         <f>'Input 1'!F40</f>
         <v>99</v>
       </c>
-      <c r="F39" s="109">
+      <c r="F39" s="190">
         <f>Estimates!D40</f>
         <v>219.78700000000001</v>
       </c>
@@ -28151,7 +28153,7 @@
         <f>'Input 1'!F41</f>
         <v>42</v>
       </c>
-      <c r="F40" s="109">
+      <c r="F40" s="190">
         <f>Estimates!D41</f>
         <v>199.36099999999999</v>
       </c>
@@ -28237,7 +28239,7 @@
         <f>'Input 1'!F42</f>
         <v>410</v>
       </c>
-      <c r="F41" s="109">
+      <c r="F41" s="190">
         <f>Estimates!D42</f>
         <v>351.69499999999999</v>
       </c>
@@ -28323,7 +28325,7 @@
         <f>'Input 1'!F43</f>
         <v>22</v>
       </c>
-      <c r="F42" s="109">
+      <c r="F42" s="190">
         <f>Estimates!D43</f>
         <v>192.101</v>
       </c>
@@ -28409,7 +28411,7 @@
         <f>'Input 1'!F44</f>
         <v>48</v>
       </c>
-      <c r="F43" s="109">
+      <c r="F43" s="190">
         <f>Estimates!D44</f>
         <v>223.78899999999999</v>
       </c>
@@ -28495,7 +28497,7 @@
         <f>'Input 1'!F45</f>
         <v>42</v>
       </c>
-      <c r="F44" s="109">
+      <c r="F44" s="190">
         <f>Estimates!D45</f>
         <v>172.768</v>
       </c>
@@ -28581,7 +28583,7 @@
         <f>'Input 1'!F46</f>
         <v>85</v>
       </c>
-      <c r="F45" s="109">
+      <c r="F45" s="190">
         <f>Estimates!D46</f>
         <v>104.842</v>
       </c>
@@ -28667,7 +28669,7 @@
         <f>'Input 1'!F47</f>
         <v>1362</v>
       </c>
-      <c r="F46" s="109">
+      <c r="F46" s="190">
         <f>Estimates!D47</f>
         <v>291.65199999999999</v>
       </c>
@@ -28753,7 +28755,7 @@
         <f>'Input 1'!F48</f>
         <v>25</v>
       </c>
-      <c r="F47" s="109">
+      <c r="F47" s="190">
         <f>Estimates!D48</f>
         <v>169.66499999999999</v>
       </c>
@@ -28839,7 +28841,7 @@
         <f>'Input 1'!F49</f>
         <v>73</v>
       </c>
-      <c r="F48" s="109">
+      <c r="F48" s="190">
         <f>Estimates!D49</f>
         <v>197.84299999999999</v>
       </c>
@@ -28925,7 +28927,7 @@
         <f>'Input 1'!F50</f>
         <v>725</v>
       </c>
-      <c r="F49" s="109">
+      <c r="F49" s="190">
         <f>Estimates!D50</f>
         <v>377.75599999999997</v>
       </c>
@@ -29011,7 +29013,7 @@
         <f>'Input 1'!F51</f>
         <v>11</v>
       </c>
-      <c r="F50" s="109">
+      <c r="F50" s="190">
         <f>Estimates!D51</f>
         <v>57.235999999999997</v>
       </c>
@@ -29097,7 +29099,7 @@
         <f>'Input 1'!F52</f>
         <v>297</v>
       </c>
-      <c r="F51" s="109">
+      <c r="F51" s="190">
         <f>Estimates!D52</f>
         <v>256.94</v>
       </c>
@@ -29183,7 +29185,7 @@
         <f>'Input 1'!F53</f>
         <v>14</v>
       </c>
-      <c r="F52" s="109">
+      <c r="F52" s="190">
         <f>Estimates!D53</f>
         <v>80.13</v>
       </c>
@@ -29269,7 +29271,7 @@
         <f>'Input 1'!F54</f>
         <v>6</v>
       </c>
-      <c r="F53" s="109">
+      <c r="F53" s="190">
         <f>Estimates!D54</f>
         <v>62.41</v>
       </c>
@@ -29355,7 +29357,7 @@
         <f>'Input 1'!F55</f>
         <v>22</v>
       </c>
-      <c r="F54" s="109">
+      <c r="F54" s="190">
         <f>Estimates!D55</f>
         <v>85.103999999999999</v>
       </c>
@@ -29441,7 +29443,7 @@
         <f>'Input 1'!F56</f>
         <v>1550</v>
       </c>
-      <c r="F55" s="109">
+      <c r="F55" s="190">
         <f>Estimates!D56</f>
         <v>2549.9940000000001</v>
       </c>
@@ -29527,7 +29529,7 @@
         <f>'Input 1'!F57</f>
         <v>1534</v>
       </c>
-      <c r="F56" s="109">
+      <c r="F56" s="190">
         <f>Estimates!D57</f>
         <v>1486.127</v>
       </c>
@@ -29613,7 +29615,7 @@
         <f>'Input 1'!F58</f>
         <v>335</v>
       </c>
-      <c r="F57" s="109">
+      <c r="F57" s="190">
         <f>Estimates!D58</f>
         <v>1283.3409999999999</v>
       </c>
@@ -29699,7 +29701,7 @@
         <f>'Input 1'!F59</f>
         <v>1874</v>
       </c>
-      <c r="F58" s="109">
+      <c r="F58" s="190">
         <f>Estimates!D59</f>
         <v>1348.6569999999999</v>
       </c>
@@ -29785,7 +29787,7 @@
         <f>'Input 1'!F60</f>
         <v>461</v>
       </c>
-      <c r="F59" s="109">
+      <c r="F59" s="190">
         <f>Estimates!D60</f>
         <v>534.78599999999994</v>
       </c>
@@ -29871,7 +29873,7 @@
         <f>'Input 1'!F61</f>
         <v>485</v>
       </c>
-      <c r="F60" s="109">
+      <c r="F60" s="190">
         <f>Estimates!D61</f>
         <v>1042.7660000000001</v>
       </c>
@@ -29957,7 +29959,7 @@
         <f>'Input 1'!F62</f>
         <v>1516</v>
       </c>
-      <c r="F61" s="109">
+      <c r="F61" s="190">
         <f>Estimates!D62</f>
         <v>1823.2339999999999</v>
       </c>
@@ -30043,7 +30045,7 @@
         <f>'Input 1'!F63</f>
         <v>239</v>
       </c>
-      <c r="F62" s="109">
+      <c r="F62" s="190">
         <f>Estimates!D63</f>
         <v>489.1</v>
       </c>
@@ -30129,7 +30131,7 @@
         <f>'Input 1'!F64</f>
         <v>1929</v>
       </c>
-      <c r="F63" s="109">
+      <c r="F63" s="190">
         <f>Estimates!D64</f>
         <v>1927.8589999999999</v>
       </c>
@@ -30215,7 +30217,7 @@
         <f>'Input 1'!F65</f>
         <v>1032</v>
       </c>
-      <c r="F64" s="109">
+      <c r="F64" s="190">
         <f>Estimates!D65</f>
         <v>591.56899999999996</v>
       </c>
@@ -30301,7 +30303,7 @@
         <f>'Input 1'!F66</f>
         <v>917</v>
       </c>
-      <c r="F65" s="109">
+      <c r="F65" s="190">
         <f>Estimates!D66</f>
         <v>1105.8</v>
       </c>
@@ -30387,7 +30389,7 @@
         <f>'Input 1'!F67</f>
         <v>688</v>
       </c>
-      <c r="F66" s="109">
+      <c r="F66" s="190">
         <f>Estimates!D67</f>
         <v>804.19299999999998</v>
       </c>
@@ -30473,7 +30475,7 @@
         <f>'Input 1'!F68</f>
         <v>615</v>
       </c>
-      <c r="F67" s="109">
+      <c r="F67" s="190">
         <f>Estimates!D68</f>
         <v>1152.528</v>
       </c>
@@ -30559,7 +30561,7 @@
         <f>'Input 1'!F69</f>
         <v>1434</v>
       </c>
-      <c r="F68" s="109">
+      <c r="F68" s="190">
         <f>Estimates!D69</f>
         <v>1153.8510000000001</v>
       </c>
@@ -30645,7 +30647,7 @@
         <f>'Input 1'!F70</f>
         <v>308</v>
       </c>
-      <c r="F69" s="109">
+      <c r="F69" s="190">
         <f>Estimates!D70</f>
         <v>896.524</v>
       </c>
@@ -30731,7 +30733,7 @@
         <f>'Input 1'!F71</f>
         <v>404</v>
       </c>
-      <c r="F70" s="109">
+      <c r="F70" s="190">
         <f>Estimates!D71</f>
         <v>674.36800000000005</v>
       </c>
@@ -30817,7 +30819,7 @@
         <f>'Input 1'!F72</f>
         <v>1533</v>
       </c>
-      <c r="F71" s="109">
+      <c r="F71" s="190">
         <f>Estimates!D72</f>
         <v>1020.675</v>
       </c>
@@ -30903,7 +30905,7 @@
         <f>'Input 1'!F73</f>
         <v>744</v>
       </c>
-      <c r="F72" s="109">
+      <c r="F72" s="190">
         <f>Estimates!D73</f>
         <v>1722.7909999999999</v>
       </c>
@@ -30989,7 +30991,7 @@
         <f>'Input 1'!F74</f>
         <v>688</v>
       </c>
-      <c r="F73" s="109">
+      <c r="F73" s="190">
         <f>Estimates!D74</f>
         <v>813.75599999999997</v>
       </c>
@@ -31075,7 +31077,7 @@
         <f>'Input 1'!F75</f>
         <v>1340</v>
       </c>
-      <c r="F74" s="109">
+      <c r="F74" s="190">
         <f>Estimates!D75</f>
         <v>1758.4159999999999</v>
       </c>
@@ -31161,7 +31163,7 @@
         <f>'Input 1'!F76</f>
         <v>2140</v>
       </c>
-      <c r="F75" s="109">
+      <c r="F75" s="190">
         <f>Estimates!D76</f>
         <v>2695.395</v>
       </c>
@@ -31247,7 +31249,7 @@
         <f>'Input 1'!F77</f>
         <v>201</v>
       </c>
-      <c r="F76" s="109">
+      <c r="F76" s="190">
         <f>Estimates!D77</f>
         <v>509.80099999999999</v>
       </c>
@@ -31333,7 +31335,7 @@
         <f>'Input 1'!F78</f>
         <v>356</v>
       </c>
-      <c r="F77" s="109">
+      <c r="F77" s="190">
         <f>Estimates!D78</f>
         <v>604.81100000000004</v>
       </c>
@@ -31419,7 +31421,7 @@
         <f>'Input 1'!F79</f>
         <v>1182</v>
       </c>
-      <c r="F78" s="109">
+      <c r="F78" s="190">
         <f>Estimates!D79</f>
         <v>1755.2829999999999</v>
       </c>
@@ -31505,7 +31507,7 @@
         <f>'Input 1'!F80</f>
         <v>285</v>
       </c>
-      <c r="F79" s="109">
+      <c r="F79" s="190">
         <f>Estimates!D80</f>
         <v>262.60000000000002</v>
       </c>
@@ -31591,7 +31593,7 @@
         <f>'Input 1'!F81</f>
         <v>7732</v>
       </c>
-      <c r="F80" s="109">
+      <c r="F80" s="190">
         <f>Estimates!D81</f>
         <v>5191.491</v>
       </c>
@@ -31677,7 +31679,7 @@
         <f>'Input 1'!F82</f>
         <v>933</v>
       </c>
-      <c r="F81" s="109">
+      <c r="F81" s="190">
         <f>Estimates!D82</f>
         <v>876.80499999999995</v>
       </c>
@@ -31763,7 +31765,7 @@
         <f>'Input 1'!F83</f>
         <v>316</v>
       </c>
-      <c r="F82" s="109">
+      <c r="F82" s="190">
         <f>Estimates!D83</f>
         <v>765.81500000000005</v>
       </c>
@@ -31849,7 +31851,7 @@
         <f>'Input 1'!F84</f>
         <v>1143</v>
       </c>
-      <c r="F83" s="109">
+      <c r="F83" s="190">
         <f>Estimates!D84</f>
         <v>1832.73</v>
       </c>
@@ -31935,7 +31937,7 @@
         <f>'Input 1'!F85</f>
         <v>1606</v>
       </c>
-      <c r="F84" s="109">
+      <c r="F84" s="190">
         <f>Estimates!D85</f>
         <v>2708.7640000000001</v>
       </c>
@@ -32021,7 +32023,7 @@
         <f>'Input 1'!F86</f>
         <v>587</v>
       </c>
-      <c r="F85" s="109">
+      <c r="F85" s="190">
         <f>Estimates!D86</f>
         <v>446.63600000000002</v>
       </c>
@@ -32107,7 +32109,7 @@
         <f>'Input 1'!F87</f>
         <v>264</v>
       </c>
-      <c r="F86" s="109">
+      <c r="F86" s="190">
         <f>Estimates!D87</f>
         <v>1078.1210000000001</v>
       </c>
@@ -32193,7 +32195,7 @@
         <f>'Input 1'!F88</f>
         <v>2764</v>
       </c>
-      <c r="F87" s="109">
+      <c r="F87" s="190">
         <f>Estimates!D88</f>
         <v>2086.7440000000001</v>
       </c>
@@ -32279,7 +32281,7 @@
         <f>'Input 1'!F89</f>
         <v>7113</v>
       </c>
-      <c r="F88" s="109">
+      <c r="F88" s="190">
         <f>Estimates!D89</f>
         <v>3285.8290000000002</v>
       </c>
@@ -32365,7 +32367,7 @@
         <f>'Input 1'!F90</f>
         <v>8135</v>
       </c>
-      <c r="F89" s="109">
+      <c r="F89" s="190">
         <f>Estimates!D90</f>
         <v>4085.7460000000001</v>
       </c>
@@ -32451,7 +32453,7 @@
         <f>'Input 1'!F91</f>
         <v>3940</v>
       </c>
-      <c r="F90" s="109">
+      <c r="F90" s="190">
         <f>Estimates!D91</f>
         <v>1858.318</v>
       </c>
@@ -32537,7 +32539,7 @@
         <f>'Input 1'!F92</f>
         <v>2579</v>
       </c>
-      <c r="F91" s="109">
+      <c r="F91" s="190">
         <f>Estimates!D92</f>
         <v>1628.338</v>
       </c>
@@ -32623,7 +32625,7 @@
         <f>'Input 1'!F93</f>
         <v>3059</v>
       </c>
-      <c r="F92" s="109">
+      <c r="F92" s="190">
         <f>Estimates!D93</f>
         <v>1501.954</v>
       </c>
@@ -32709,7 +32711,7 @@
         <f>'Input 1'!F94</f>
         <v>7997</v>
       </c>
-      <c r="F93" s="109">
+      <c r="F93" s="190">
         <f>Estimates!D94</f>
         <v>3326.4369999999999</v>
       </c>
@@ -32795,7 +32797,7 @@
         <f>'Input 1'!F95</f>
         <v>13606</v>
       </c>
-      <c r="F94" s="109">
+      <c r="F94" s="190">
         <f>Estimates!D95</f>
         <v>8680.6560000000009</v>
       </c>
@@ -32881,7 +32883,7 @@
         <f>'Input 1'!F96</f>
         <v>10434</v>
       </c>
-      <c r="F95" s="109">
+      <c r="F95" s="190">
         <f>Estimates!D96</f>
         <v>5552.3789999999999</v>
       </c>
@@ -32967,7 +32969,7 @@
         <f>'Input 1'!F97</f>
         <v>2920</v>
       </c>
-      <c r="F96" s="109">
+      <c r="F96" s="190">
         <f>Estimates!D97</f>
         <v>2979.366</v>
       </c>
@@ -33053,7 +33055,7 @@
         <f>'Input 1'!F98</f>
         <v>2211</v>
       </c>
-      <c r="F97" s="109">
+      <c r="F97" s="190">
         <f>Estimates!D98</f>
         <v>1261.1769999999999</v>
       </c>
@@ -33139,7 +33141,7 @@
         <f>'Input 1'!F99</f>
         <v>6667</v>
       </c>
-      <c r="F98" s="109">
+      <c r="F98" s="190">
         <f>Estimates!D99</f>
         <v>3034.8969999999999</v>
       </c>
@@ -33225,7 +33227,7 @@
         <f>'Input 1'!F100</f>
         <v>3121</v>
       </c>
-      <c r="F99" s="109">
+      <c r="F99" s="190">
         <f>Estimates!D100</f>
         <v>1311.3119999999999</v>
       </c>
@@ -33311,7 +33313,7 @@
         <f>'Input 1'!F101</f>
         <v>8284</v>
       </c>
-      <c r="F100" s="109">
+      <c r="F100" s="190">
         <f>Estimates!D101</f>
         <v>3820.2080000000001</v>
       </c>
@@ -33397,7 +33399,7 @@
         <f>'Input 1'!F102</f>
         <v>5930</v>
       </c>
-      <c r="F101" s="109">
+      <c r="F101" s="190">
         <f>Estimates!D102</f>
         <v>3199.3139999999999</v>
       </c>
@@ -33483,7 +33485,7 @@
         <f>'Input 1'!F103</f>
         <v>3301</v>
       </c>
-      <c r="F102" s="109">
+      <c r="F102" s="190">
         <f>Estimates!D103</f>
         <v>1403.597</v>
       </c>
@@ -33569,7 +33571,7 @@
         <f>'Input 1'!F104</f>
         <v>18445</v>
       </c>
-      <c r="F103" s="109">
+      <c r="F103" s="190">
         <f>Estimates!D104</f>
         <v>12898.414000000001</v>
       </c>
@@ -33655,7 +33657,7 @@
         <f>'Input 1'!F105</f>
         <v>2960</v>
       </c>
-      <c r="F104" s="109">
+      <c r="F104" s="190">
         <f>Estimates!D105</f>
         <v>2073.0259999999998</v>
       </c>
@@ -33741,7 +33743,7 @@
         <f>'Input 1'!F106</f>
         <v>3137</v>
       </c>
-      <c r="F105" s="109">
+      <c r="F105" s="190">
         <f>Estimates!D106</f>
         <v>1874.8620000000001</v>
       </c>
@@ -33827,7 +33829,7 @@
         <f>'Input 1'!F107</f>
         <v>4224</v>
       </c>
-      <c r="F106" s="109">
+      <c r="F106" s="190">
         <f>Estimates!D107</f>
         <v>1731.702</v>
       </c>
@@ -33913,7 +33915,7 @@
         <f>'Input 1'!F108</f>
         <v>4001</v>
       </c>
-      <c r="F107" s="109">
+      <c r="F107" s="190">
         <f>Estimates!D108</f>
         <v>1708.6869999999999</v>
       </c>
@@ -33999,7 +34001,7 @@
         <f>'Input 1'!F109</f>
         <v>10395</v>
       </c>
-      <c r="F108" s="109">
+      <c r="F108" s="190">
         <f>Estimates!D109</f>
         <v>5298.3180000000002</v>
       </c>
@@ -34085,7 +34087,7 @@
         <f>'Input 1'!F110</f>
         <v>10261</v>
       </c>
-      <c r="F109" s="109">
+      <c r="F109" s="190">
         <f>Estimates!D110</f>
         <v>4921.0450000000001</v>
       </c>
@@ -34171,7 +34173,7 @@
         <f>'Input 1'!F111</f>
         <v>3555</v>
       </c>
-      <c r="F110" s="109">
+      <c r="F110" s="190">
         <f>Estimates!D111</f>
         <v>1452.5830000000001</v>
       </c>
@@ -34257,7 +34259,7 @@
         <f>'Input 1'!F112</f>
         <v>2148</v>
       </c>
-      <c r="F111" s="109">
+      <c r="F111" s="190">
         <f>Estimates!D112</f>
         <v>1850.0740000000001</v>
       </c>
@@ -34343,7 +34345,7 @@
         <f>'Input 1'!F113</f>
         <v>6522</v>
       </c>
-      <c r="F112" s="109">
+      <c r="F112" s="190">
         <f>Estimates!D113</f>
         <v>3295.0360000000001</v>
       </c>
@@ -34429,7 +34431,7 @@
         <f>'Input 1'!F114</f>
         <v>4369</v>
       </c>
-      <c r="F113" s="109">
+      <c r="F113" s="190">
         <f>Estimates!D114</f>
         <v>1998.7360000000001</v>
       </c>
@@ -34515,7 +34517,7 @@
         <f>'Input 1'!F115</f>
         <v>9188</v>
       </c>
-      <c r="F114" s="109">
+      <c r="F114" s="190">
         <f>Estimates!D115</f>
         <v>5529.4690000000001</v>
       </c>
@@ -34601,7 +34603,7 @@
         <f>'Input 1'!F116</f>
         <v>3251</v>
       </c>
-      <c r="F115" s="109">
+      <c r="F115" s="190">
         <f>Estimates!D116</f>
         <v>2331.89</v>
       </c>
@@ -34687,7 +34689,7 @@
         <f>'Input 1'!F117</f>
         <v>8556</v>
       </c>
-      <c r="F116" s="109">
+      <c r="F116" s="190">
         <f>Estimates!D117</f>
         <v>6121.9470000000001</v>
       </c>
@@ -34773,7 +34775,7 @@
         <f>'Input 1'!F118</f>
         <v>4660</v>
       </c>
-      <c r="F117" s="109">
+      <c r="F117" s="190">
         <f>Estimates!D118</f>
         <v>2732.2269999999999</v>
       </c>
@@ -34859,7 +34861,7 @@
         <f>'Input 1'!F119</f>
         <v>10749</v>
       </c>
-      <c r="F118" s="109">
+      <c r="F118" s="190">
         <f>Estimates!D119</f>
         <v>4037.21</v>
       </c>
@@ -34945,7 +34947,7 @@
         <f>'Input 1'!F120</f>
         <v>5499</v>
       </c>
-      <c r="F119" s="109">
+      <c r="F119" s="190">
         <f>Estimates!D120</f>
         <v>3861.97</v>
       </c>
@@ -35031,7 +35033,7 @@
         <f>'Input 1'!F121</f>
         <v>8127</v>
       </c>
-      <c r="F120" s="109">
+      <c r="F120" s="190">
         <f>Estimates!D121</f>
         <v>4275.7979999999998</v>
       </c>
@@ -35117,7 +35119,7 @@
         <f>'Input 1'!F122</f>
         <v>4211</v>
       </c>
-      <c r="F121" s="109">
+      <c r="F121" s="190">
         <f>Estimates!D122</f>
         <v>2369.7469999999998</v>
       </c>
@@ -35203,7 +35205,7 @@
         <f>'Input 1'!F123</f>
         <v>5989</v>
       </c>
-      <c r="F122" s="109">
+      <c r="F122" s="190">
         <f>Estimates!D123</f>
         <v>3156.8980000000001</v>
       </c>
@@ -35289,7 +35291,7 @@
         <f>'Input 1'!F124</f>
         <v>3367</v>
       </c>
-      <c r="F123" s="109">
+      <c r="F123" s="190">
         <f>Estimates!D124</f>
         <v>2051.623</v>
       </c>
@@ -35375,7 +35377,7 @@
         <f>'Input 1'!F125</f>
         <v>3569</v>
       </c>
-      <c r="F124" s="109">
+      <c r="F124" s="190">
         <f>Estimates!D125</f>
         <v>3187.1170000000002</v>
       </c>
@@ -35461,7 +35463,7 @@
         <f>'Input 1'!F126</f>
         <v>2025</v>
       </c>
-      <c r="F125" s="109">
+      <c r="F125" s="190">
         <f>Estimates!D126</f>
         <v>1694.0719999999999</v>
       </c>
@@ -35547,7 +35549,7 @@
         <f>'Input 1'!F127</f>
         <v>2401</v>
       </c>
-      <c r="F126" s="109">
+      <c r="F126" s="190">
         <f>Estimates!D127</f>
         <v>3476.5770000000002</v>
       </c>
@@ -35633,7 +35635,7 @@
         <f>'Input 1'!F128</f>
         <v>2490</v>
       </c>
-      <c r="F127" s="109">
+      <c r="F127" s="190">
         <f>Estimates!D128</f>
         <v>1891.915</v>
       </c>
@@ -35719,7 +35721,7 @@
         <f>'Input 1'!F129</f>
         <v>4456</v>
       </c>
-      <c r="F128" s="109">
+      <c r="F128" s="190">
         <f>Estimates!D129</f>
         <v>2434.3429999999998</v>
       </c>
@@ -35805,7 +35807,7 @@
         <f>'Input 1'!F130</f>
         <v>1551</v>
       </c>
-      <c r="F129" s="109">
+      <c r="F129" s="190">
         <f>Estimates!D130</f>
         <v>1095.867</v>
       </c>
@@ -35891,7 +35893,7 @@
         <f>'Input 1'!F131</f>
         <v>3129</v>
       </c>
-      <c r="F130" s="109">
+      <c r="F130" s="190">
         <f>Estimates!D131</f>
         <v>1142.9649999999999</v>
       </c>
@@ -35977,7 +35979,7 @@
         <f>'Input 1'!F132</f>
         <v>1421</v>
       </c>
-      <c r="F131" s="109">
+      <c r="F131" s="190">
         <f>Estimates!D132</f>
         <v>1478.443</v>
       </c>
@@ -36063,7 +36065,7 @@
         <f>'Input 1'!F133</f>
         <v>1265</v>
       </c>
-      <c r="F132" s="109">
+      <c r="F132" s="190">
         <f>Estimates!D133</f>
         <v>1234.0989999999999</v>
       </c>
@@ -36149,7 +36151,7 @@
         <f>'Input 1'!F134</f>
         <v>3472</v>
       </c>
-      <c r="F133" s="109">
+      <c r="F133" s="190">
         <f>Estimates!D134</f>
         <v>2699.1179999999999</v>
       </c>
@@ -36235,7 +36237,7 @@
         <f>'Input 1'!F135</f>
         <v>2758</v>
       </c>
-      <c r="F134" s="109">
+      <c r="F134" s="190">
         <f>Estimates!D135</f>
         <v>2767.7080000000001</v>
       </c>
@@ -36321,7 +36323,7 @@
         <f>'Input 1'!F136</f>
         <v>2896</v>
       </c>
-      <c r="F135" s="109">
+      <c r="F135" s="190">
         <f>Estimates!D136</f>
         <v>1702.1120000000001</v>
       </c>
@@ -36407,7 +36409,7 @@
         <f>'Input 1'!F137</f>
         <v>2198</v>
       </c>
-      <c r="F136" s="109">
+      <c r="F136" s="190">
         <f>Estimates!D137</f>
         <v>2427.7289999999998</v>
       </c>
@@ -36493,7 +36495,7 @@
         <f>'Input 1'!F138</f>
         <v>1316</v>
       </c>
-      <c r="F137" s="109">
+      <c r="F137" s="190">
         <f>Estimates!D138</f>
         <v>864.09699999999998</v>
       </c>
@@ -36579,7 +36581,7 @@
         <f>'Input 1'!F139</f>
         <v>3313</v>
       </c>
-      <c r="F138" s="109">
+      <c r="F138" s="190">
         <f>Estimates!D139</f>
         <v>1674.05</v>
       </c>
@@ -36665,7 +36667,7 @@
         <f>'Input 1'!F140</f>
         <v>2688</v>
       </c>
-      <c r="F139" s="109">
+      <c r="F139" s="190">
         <f>Estimates!D140</f>
         <v>1788.058</v>
       </c>
@@ -36751,7 +36753,7 @@
         <f>'Input 1'!F141</f>
         <v>3806</v>
       </c>
-      <c r="F140" s="109">
+      <c r="F140" s="190">
         <f>Estimates!D141</f>
         <v>2311.52</v>
       </c>
@@ -36837,7 +36839,7 @@
         <f>'Input 1'!F142</f>
         <v>4196</v>
       </c>
-      <c r="F141" s="109">
+      <c r="F141" s="190">
         <f>Estimates!D142</f>
         <v>1782.46</v>
       </c>
@@ -36923,7 +36925,7 @@
         <f>'Input 1'!F143</f>
         <v>1669</v>
       </c>
-      <c r="F142" s="109">
+      <c r="F142" s="190">
         <f>Estimates!D143</f>
         <v>1345.0550000000001</v>
       </c>
@@ -37009,7 +37011,7 @@
         <f>'Input 1'!F144</f>
         <v>3158</v>
       </c>
-      <c r="F143" s="109">
+      <c r="F143" s="190">
         <f>Estimates!D144</f>
         <v>1885.0139999999999</v>
       </c>
@@ -37095,7 +37097,7 @@
         <f>'Input 1'!F145</f>
         <v>981</v>
       </c>
-      <c r="F144" s="109">
+      <c r="F144" s="190">
         <f>Estimates!D145</f>
         <v>873.13300000000004</v>
       </c>
@@ -37181,7 +37183,7 @@
         <f>'Input 1'!F146</f>
         <v>3088</v>
       </c>
-      <c r="F145" s="109">
+      <c r="F145" s="190">
         <f>Estimates!D146</f>
         <v>1682.605</v>
       </c>
@@ -37267,7 +37269,7 @@
         <f>'Input 1'!F147</f>
         <v>886</v>
       </c>
-      <c r="F146" s="109">
+      <c r="F146" s="190">
         <f>Estimates!D147</f>
         <v>961.26599999999996</v>
       </c>
@@ -37353,7 +37355,7 @@
         <f>'Input 1'!F148</f>
         <v>1381</v>
       </c>
-      <c r="F147" s="109">
+      <c r="F147" s="190">
         <f>Estimates!D148</f>
         <v>759.14599999999996</v>
       </c>
@@ -37439,7 +37441,7 @@
         <f>'Input 1'!F149</f>
         <v>1945</v>
       </c>
-      <c r="F148" s="109">
+      <c r="F148" s="190">
         <f>Estimates!D149</f>
         <v>1926.375</v>
       </c>
@@ -37525,7 +37527,7 @@
         <f>'Input 1'!F150</f>
         <v>938</v>
       </c>
-      <c r="F149" s="109">
+      <c r="F149" s="190">
         <f>Estimates!D150</f>
         <v>1114.5340000000001</v>
       </c>
@@ -37611,7 +37613,7 @@
         <f>'Input 1'!F151</f>
         <v>3414</v>
       </c>
-      <c r="F150" s="109">
+      <c r="F150" s="190">
         <f>Estimates!D151</f>
         <v>1217.1300000000001</v>
       </c>
@@ -37697,7 +37699,7 @@
         <f>'Input 1'!F152</f>
         <v>2853</v>
       </c>
-      <c r="F151" s="109">
+      <c r="F151" s="190">
         <f>Estimates!D152</f>
         <v>4615.9089999999997</v>
       </c>

</xml_diff>